<commit_message>
Excel URLs (espace Client)
</commit_message>
<xml_diff>
--- a/WS_Rest.xlsx
+++ b/WS_Rest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="28515" windowHeight="12840"/>
@@ -11,12 +11,12 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>VERBE</t>
   </si>
@@ -65,14 +65,307 @@
         <scheme val="minor"/>
       </rPr>
       <t>/client/comptes/{RIB}</t>
+    </r>
+  </si>
+  <si>
+    <t>getAllNotifications()</t>
+  </si>
+  <si>
+    <t>List&lt;Notification&gt;</t>
+  </si>
+  <si>
+    <t>exemple</t>
+  </si>
+  <si>
+    <t>ajouterNotification()</t>
+  </si>
+  <si>
+    <t>supprimerNotification()</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>endpoint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/client/{id}/comptes</t>
+    </r>
+  </si>
+  <si>
+    <t>getAllComptes()</t>
+  </si>
+  <si>
+    <t>getCompteById()</t>
+  </si>
+  <si>
+    <t>Compte</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>endpoint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/client/{id}/compte/{IBAN}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>endpoint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/client/{id}/notifications</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>endpoint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/client/{id}/notifications/ajout</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>endpoint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/client/{id}/notification/{id}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>endpoint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/client/{id}/compte/{IBAN}/operations</t>
+    </r>
+  </si>
+  <si>
+    <t>getAllOperations()</t>
+  </si>
+  <si>
+    <t>List&lt;Operation&gt;</t>
+  </si>
+  <si>
+    <t>getAllOperations(int duree)</t>
+  </si>
+  <si>
+    <t>getAllOperations(Date dateDebut, Date dateFin)</t>
+  </si>
+  <si>
+    <t>getAllOperations(Date dateDebut)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>endpoint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/client/{id}/compte/{IBAN}/operations (+param)</t>
+    </r>
+  </si>
+  <si>
+    <t>ajouterOperation()</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>endpoint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/client/{id}/compte/{IBAN}/operation/ajout</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>endpoint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/client/{id}/compte/{IBAN}/chequier</t>
+    </r>
+  </si>
+  <si>
+    <t>ajoutDemandeChequier()</t>
+  </si>
+  <si>
+    <t>ajoutDemandeCompte()</t>
+  </si>
+  <si>
+    <t>Demande</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>endpoint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/client/{id}/comptes/ajout</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,7 +502,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -244,7 +536,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -420,53 +711,257 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
-    <col min="3" max="3" width="58.42578125" customWidth="1"/>
-    <col min="4" max="4" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="63.85546875" customWidth="1"/>
+    <col min="4" max="4" width="58.42578125" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>7</v>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -476,24 +971,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>